<commit_message>
module col dynamic change
</commit_message>
<xml_diff>
--- a/testData/Notification/WF1_Send_Notify_ETR_S_Test.xlsx
+++ b/testData/Notification/WF1_Send_Notify_ETR_S_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>WorkflowName</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>93176</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
         <v>48</v>
       </c>
       <c r="AK2" t="s" s="0">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
ExecuteTask In Progress Test 1
</commit_message>
<xml_diff>
--- a/testData/Notification/WF1_Send_Notify_ETR_S_Test.xlsx
+++ b/testData/Notification/WF1_Send_Notify_ETR_S_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
   <si>
     <t>WorkflowName</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>123113</t>
+  </si>
+  <si>
+    <t>123433</t>
+  </si>
+  <si>
+    <t>123437</t>
+  </si>
+  <si>
+    <t>123441</t>
   </si>
 </sst>
 </file>
@@ -658,7 +667,7 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AK2" t="s" s="0">
         <v>29</v>
@@ -790,7 +799,7 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>1</v>
@@ -915,7 +924,7 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>1</v>
@@ -1040,7 +1049,7 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AQ2" s="3" t="s">
         <v>1</v>

</xml_diff>